<commit_message>
Changes to import and home page to account for other leagues.
</commit_message>
<xml_diff>
--- a/static/mlb-2023-player-picks.xlsx
+++ b/static/mlb-2023-player-picks.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/tql/Projects/python/over-under/static/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A7175EA3-7A7C-3C4F-9316-C8A920112FDB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B3E604CD-E6E2-274B-99DC-F8FDA2CF542E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="17500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="17500" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Picks" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="493" uniqueCount="91">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="525" uniqueCount="92">
   <si>
     <t>Player</t>
   </si>
@@ -307,6 +307,9 @@
   </si>
   <si>
     <t>MLB</t>
+  </si>
+  <si>
+    <t>Year</t>
   </si>
 </sst>
 </file>
@@ -589,7 +592,7 @@
   </sheetPr>
   <dimension ref="A1:K46"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="J14" sqref="J14"/>
     </sheetView>
   </sheetViews>
@@ -2218,263 +2221,449 @@
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
-  <dimension ref="A1:B34"/>
+  <dimension ref="A1:D34"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A31" sqref="A31"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E24" sqref="E24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="12.6640625" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
   <sheetData>
-    <row r="1" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="1" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A1" s="1" t="s">
         <v>48</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>49</v>
       </c>
-    </row>
-    <row r="2" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="C1" s="3" t="s">
+        <v>50</v>
+      </c>
+      <c r="D1" s="3" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A2" s="4" t="s">
         <v>31</v>
       </c>
       <c r="B2" s="1">
         <v>95</v>
       </c>
-    </row>
-    <row r="3" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="C2" s="3" t="s">
+        <v>90</v>
+      </c>
+      <c r="D2">
+        <v>2023</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A3" s="4" t="s">
         <v>52</v>
       </c>
       <c r="B3" s="1">
         <v>95</v>
       </c>
-    </row>
-    <row r="4" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="C3" s="3" t="s">
+        <v>90</v>
+      </c>
+      <c r="D3">
+        <v>2023</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A4" s="4" t="s">
         <v>65</v>
       </c>
       <c r="B4" s="1">
         <v>94</v>
       </c>
-    </row>
-    <row r="5" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="C4" s="3" t="s">
+        <v>90</v>
+      </c>
+      <c r="D4">
+        <v>2023</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A5" s="4" t="s">
         <v>53</v>
       </c>
       <c r="B5" s="1">
         <v>92</v>
       </c>
-    </row>
-    <row r="6" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="C5" s="3" t="s">
+        <v>90</v>
+      </c>
+      <c r="D5">
+        <v>2023</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A6" s="4" t="s">
         <v>54</v>
       </c>
       <c r="B6" s="1">
         <v>89</v>
       </c>
-    </row>
-    <row r="7" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="C6" s="3" t="s">
+        <v>90</v>
+      </c>
+      <c r="D6">
+        <v>2023</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A7" s="4" t="s">
         <v>17</v>
       </c>
       <c r="B7" s="1">
         <v>88</v>
       </c>
-    </row>
-    <row r="8" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="C7" s="3" t="s">
+        <v>90</v>
+      </c>
+      <c r="D7">
+        <v>2023</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A8" s="4" t="s">
         <v>55</v>
       </c>
       <c r="B8" s="1">
         <v>85</v>
       </c>
-    </row>
-    <row r="9" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="C8" s="3" t="s">
+        <v>90</v>
+      </c>
+      <c r="D8">
+        <v>2023</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A9" s="4" t="s">
         <v>38</v>
       </c>
       <c r="B9" s="1">
         <v>81</v>
       </c>
-    </row>
-    <row r="10" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="C9" s="3" t="s">
+        <v>90</v>
+      </c>
+      <c r="D9">
+        <v>2023</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A10" s="4" t="s">
         <v>56</v>
       </c>
       <c r="B10" s="1">
         <v>77</v>
       </c>
-    </row>
-    <row r="11" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="C10" s="3" t="s">
+        <v>90</v>
+      </c>
+      <c r="D10">
+        <v>2023</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A11" s="4" t="s">
         <v>23</v>
       </c>
       <c r="B11" s="1">
         <v>76</v>
       </c>
-    </row>
-    <row r="12" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="C11" s="3" t="s">
+        <v>90</v>
+      </c>
+      <c r="D11">
+        <v>2023</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A12" s="4" t="s">
         <v>21</v>
       </c>
       <c r="B12" s="1">
         <v>75</v>
       </c>
-    </row>
-    <row r="13" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="C12" s="3" t="s">
+        <v>90</v>
+      </c>
+      <c r="D12">
+        <v>2023</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A13" s="4" t="s">
         <v>11</v>
       </c>
       <c r="B13" s="1">
         <v>66</v>
       </c>
-    </row>
-    <row r="14" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="C13" s="3" t="s">
+        <v>90</v>
+      </c>
+      <c r="D13">
+        <v>2023</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A14" s="4" t="s">
         <v>16</v>
       </c>
       <c r="B14" s="1">
         <v>67</v>
       </c>
-    </row>
-    <row r="15" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="C14" s="3" t="s">
+        <v>90</v>
+      </c>
+      <c r="D14">
+        <v>2023</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A15" s="4" t="s">
         <v>57</v>
       </c>
       <c r="B15" s="1">
         <v>66</v>
       </c>
-    </row>
-    <row r="16" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="C15" s="3" t="s">
+        <v>90</v>
+      </c>
+      <c r="D15">
+        <v>2023</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A16" s="4" t="s">
         <v>26</v>
       </c>
       <c r="B16" s="1">
         <v>60</v>
       </c>
-    </row>
-    <row r="17" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="C16" s="3" t="s">
+        <v>90</v>
+      </c>
+      <c r="D16">
+        <v>2023</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A17" s="4" t="s">
         <v>32</v>
       </c>
       <c r="B17" s="1">
         <v>95</v>
       </c>
-    </row>
-    <row r="18" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="C17" s="3" t="s">
+        <v>90</v>
+      </c>
+      <c r="D17">
+        <v>2023</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A18" s="4" t="s">
         <v>58</v>
       </c>
       <c r="B18" s="1">
         <v>94</v>
       </c>
-    </row>
-    <row r="19" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="C18" s="3" t="s">
+        <v>90</v>
+      </c>
+      <c r="D18">
+        <v>2023</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A19" s="4" t="s">
         <v>59</v>
       </c>
       <c r="B19" s="2">
         <v>92</v>
       </c>
-    </row>
-    <row r="20" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="C19" s="3" t="s">
+        <v>90</v>
+      </c>
+      <c r="D19">
+        <v>2023</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A20" s="4" t="s">
         <v>18</v>
       </c>
       <c r="B20" s="2">
         <v>89</v>
       </c>
-    </row>
-    <row r="21" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="C20" s="3" t="s">
+        <v>90</v>
+      </c>
+      <c r="D20">
+        <v>2023</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A21" s="4" t="s">
         <v>13</v>
       </c>
       <c r="B21" s="2">
         <v>88</v>
       </c>
-    </row>
-    <row r="22" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="C21" s="3" t="s">
+        <v>90</v>
+      </c>
+      <c r="D21">
+        <v>2023</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A22" s="4" t="s">
         <v>35</v>
       </c>
       <c r="B22" s="2">
         <v>87</v>
       </c>
-    </row>
-    <row r="23" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="C22" s="3" t="s">
+        <v>90</v>
+      </c>
+      <c r="D22">
+        <v>2023</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A23" s="4" t="s">
         <v>60</v>
       </c>
       <c r="B23" s="2">
         <v>83</v>
       </c>
-    </row>
-    <row r="24" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="C23" s="3" t="s">
+        <v>90</v>
+      </c>
+      <c r="D23">
+        <v>2023</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A24" s="4" t="s">
         <v>12</v>
       </c>
       <c r="B24" s="2">
         <v>83</v>
       </c>
-    </row>
-    <row r="25" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="C24" s="3" t="s">
+        <v>90</v>
+      </c>
+      <c r="D24">
+        <v>2023</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A25" s="4" t="s">
         <v>61</v>
       </c>
       <c r="B25" s="2">
         <v>82</v>
       </c>
-    </row>
-    <row r="26" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="C25" s="3" t="s">
+        <v>90</v>
+      </c>
+      <c r="D25">
+        <v>2023</v>
+      </c>
+    </row>
+    <row r="26" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A26" s="4" t="s">
         <v>62</v>
       </c>
       <c r="B26" s="2">
         <v>80</v>
       </c>
-    </row>
-    <row r="27" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="C26" s="3" t="s">
+        <v>90</v>
+      </c>
+      <c r="D26">
+        <v>2023</v>
+      </c>
+    </row>
+    <row r="27" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A27" s="4" t="s">
         <v>63</v>
       </c>
       <c r="B27" s="2">
         <v>77</v>
       </c>
-    </row>
-    <row r="28" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="C27" s="3" t="s">
+        <v>90</v>
+      </c>
+      <c r="D27">
+        <v>2023</v>
+      </c>
+    </row>
+    <row r="28" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A28" s="4" t="s">
         <v>27</v>
       </c>
       <c r="B28" s="2">
         <v>77</v>
       </c>
-    </row>
-    <row r="29" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="C28" s="3" t="s">
+        <v>90</v>
+      </c>
+      <c r="D28">
+        <v>2023</v>
+      </c>
+    </row>
+    <row r="29" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A29" s="4" t="s">
         <v>39</v>
       </c>
       <c r="B29" s="2">
         <v>70</v>
       </c>
-    </row>
-    <row r="30" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="C29" s="3" t="s">
+        <v>90</v>
+      </c>
+      <c r="D29">
+        <v>2023</v>
+      </c>
+    </row>
+    <row r="30" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A30" s="4" t="s">
         <v>15</v>
       </c>
       <c r="B30" s="2">
         <v>68</v>
       </c>
-    </row>
-    <row r="31" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="C30" s="3" t="s">
+        <v>90</v>
+      </c>
+      <c r="D30">
+        <v>2023</v>
+      </c>
+    </row>
+    <row r="31" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A31" s="4" t="s">
         <v>64</v>
       </c>
       <c r="B31" s="2">
         <v>59</v>
       </c>
-    </row>
-    <row r="32" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="C31" s="3" t="s">
+        <v>90</v>
+      </c>
+      <c r="D31">
+        <v>2023</v>
+      </c>
+    </row>
+    <row r="32" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A32" s="1"/>
       <c r="B32" s="2"/>
     </row>

</xml_diff>